<commit_message>
updated value set parser to handle new MAT valueset format
</commit_message>
<xml_diff>
--- a/test/fixtures/white_list.xlsx
+++ b/test/fixtures/white_list.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
-    <sheet name="Disclaimer" sheetId="5" r:id="rId1"/>
-    <sheet name="White_List" sheetId="4" r:id="rId2"/>
-    <sheet name="Supplemental Value Sets" sheetId="6" r:id="rId3"/>
+    <sheet name="White_List" sheetId="4" r:id="rId1"/>
+    <sheet name="Supplemental Value Sets" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>ICD-9</t>
   </si>
@@ -42,9 +41,6 @@
   </si>
   <si>
     <t>Value Set Name</t>
-  </si>
-  <si>
-    <t>QDM Category</t>
   </si>
   <si>
     <t>Code System</t>
@@ -72,9 +68,6 @@
   </si>
   <si>
     <t>07/26/2012 02:27 PM</t>
-  </si>
-  <si>
-    <t>Condition/Diagnosis/Problem</t>
   </si>
   <si>
     <t>Grouping</t>
@@ -1954,27 +1947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K203"/>
+  <dimension ref="A1:J203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1983,17 +1959,16 @@
     <col min="2" max="2" width="41.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="2" customWidth="1"/>
     <col min="4" max="4" width="39.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.5" style="5" customWidth="1"/>
-    <col min="9" max="9" width="77.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="2"/>
-    <col min="11" max="11" width="33.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.5" style="5" customWidth="1"/>
+    <col min="8" max="8" width="77.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="2"/>
+    <col min="10" max="10" width="33.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2012,523 +1987,472 @@
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:10">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12" s="7"/>
-      <c r="I12"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="G12" s="7"/>
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13" s="7"/>
-      <c r="I13"/>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="G13" s="7"/>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15" s="7"/>
-      <c r="I15"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="G15" s="7"/>
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16" s="7"/>
-      <c r="I16"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="G16" s="7"/>
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17" s="7"/>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="G17" s="7"/>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18" s="7"/>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="G18" s="7"/>
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19" s="7"/>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="G19" s="7"/>
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20" s="7"/>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="G20" s="7"/>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21" s="7"/>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="G21" s="7"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22" s="7"/>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="G22" s="7"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23" s="12"/>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="G23" s="12"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24" s="7"/>
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="G24" s="7"/>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25" s="7"/>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="G25" s="7"/>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26" s="7"/>
-      <c r="I26"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="G26" s="7"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27" s="7"/>
-      <c r="I27"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="G27" s="7"/>
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28" s="7"/>
-      <c r="I28"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="G28" s="7"/>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29" s="7"/>
-      <c r="I29"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="G29" s="7"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30" s="7"/>
-      <c r="I30"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="G30" s="7"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31" s="7"/>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="G31" s="7"/>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32" s="7"/>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="G32" s="7"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33" s="7"/>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="G33" s="7"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
       <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34" s="7"/>
-      <c r="I34"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="G34" s="7"/>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
       <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35" s="7"/>
-      <c r="I35"/>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="G35" s="7"/>
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
       <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36" s="7"/>
-      <c r="I36"/>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="G36" s="7"/>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
       <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37" s="7"/>
-      <c r="I37"/>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="G37" s="7"/>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
       <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38" s="7"/>
-      <c r="I38"/>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="G38" s="7"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
       <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39" s="7"/>
-      <c r="I39"/>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="G39" s="7"/>
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40" s="7"/>
-      <c r="I40"/>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="G40" s="7"/>
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41" s="7"/>
-      <c r="I41"/>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="G41" s="7"/>
+      <c r="H41"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -2537,9 +2461,8 @@
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
-      <c r="I42"/>
-    </row>
-    <row r="43" spans="1:9">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -2548,9 +2471,8 @@
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
-      <c r="I43"/>
-    </row>
-    <row r="44" spans="1:9">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -2559,9 +2481,8 @@
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
-      <c r="I44"/>
-    </row>
-    <row r="45" spans="1:9">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -2570,9 +2491,8 @@
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
-      <c r="I45"/>
-    </row>
-    <row r="46" spans="1:9">
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -2581,9 +2501,8 @@
       <c r="F46"/>
       <c r="G46"/>
       <c r="H46"/>
-      <c r="I46"/>
-    </row>
-    <row r="47" spans="1:9">
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -2592,9 +2511,8 @@
       <c r="F47"/>
       <c r="G47"/>
       <c r="H47"/>
-      <c r="I47"/>
-    </row>
-    <row r="48" spans="1:9">
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -2603,9 +2521,8 @@
       <c r="F48"/>
       <c r="G48"/>
       <c r="H48"/>
-      <c r="I48"/>
-    </row>
-    <row r="49" spans="1:9">
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -2614,174 +2531,158 @@
       <c r="F49"/>
       <c r="G49"/>
       <c r="H49"/>
-      <c r="I49"/>
-    </row>
-    <row r="50" spans="1:9" ht="15">
+    </row>
+    <row r="50" spans="1:8" ht="15">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="8"/>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="G50" s="10"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
       <c r="E51"/>
       <c r="F51"/>
-      <c r="G51"/>
-      <c r="H51" s="7"/>
-      <c r="I51"/>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="G51" s="7"/>
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
       <c r="F52"/>
-      <c r="G52"/>
-      <c r="H52" s="7"/>
-      <c r="I52"/>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="G52" s="7"/>
+      <c r="H52"/>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
       <c r="E53"/>
       <c r="F53"/>
-      <c r="G53"/>
-      <c r="H53" s="7"/>
-      <c r="I53"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="G53" s="7"/>
+      <c r="H53"/>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
       <c r="F54"/>
-      <c r="G54"/>
-      <c r="H54" s="7"/>
-      <c r="I54"/>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="G54" s="7"/>
+      <c r="H54"/>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
       <c r="E55"/>
       <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55" s="7"/>
-      <c r="I55"/>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="G55" s="7"/>
+      <c r="H55"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
       <c r="E56"/>
       <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56" s="7"/>
-      <c r="I56"/>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="G56" s="7"/>
+      <c r="H56"/>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
       <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57" s="7"/>
-      <c r="I57"/>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="G57" s="7"/>
+      <c r="H57"/>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
       <c r="E58"/>
       <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58" s="12"/>
-      <c r="I58"/>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="G58" s="12"/>
+      <c r="H58"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
       <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59" s="7"/>
-      <c r="I59"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="G59" s="7"/>
+      <c r="H59"/>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60" s="7"/>
-      <c r="I60"/>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="G60" s="7"/>
+      <c r="H60"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61" s="7"/>
-      <c r="I61"/>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="G61" s="7"/>
+      <c r="H61"/>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
       <c r="E62"/>
       <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62" s="7"/>
-      <c r="I62"/>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="G62" s="7"/>
+      <c r="H62"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
       <c r="E63"/>
       <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63" s="7"/>
-      <c r="I63"/>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="G63" s="7"/>
+      <c r="H63"/>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
       <c r="E64"/>
       <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64" s="7"/>
-      <c r="I64"/>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="G64" s="7"/>
+      <c r="H64"/>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -2790,581 +2691,528 @@
       <c r="F65"/>
       <c r="G65"/>
       <c r="H65"/>
-      <c r="I65"/>
-    </row>
-    <row r="66" spans="1:9">
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
       <c r="E66"/>
       <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66" s="7"/>
-      <c r="I66"/>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="G66" s="7"/>
+      <c r="H66"/>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
       <c r="E67"/>
       <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67" s="7"/>
-      <c r="I67"/>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="G67" s="7"/>
+      <c r="H67"/>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
       <c r="E68"/>
       <c r="F68"/>
-      <c r="G68"/>
-      <c r="H68" s="7"/>
-      <c r="I68"/>
-    </row>
-    <row r="69" spans="1:9">
+      <c r="G68" s="7"/>
+      <c r="H68"/>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
       <c r="E69"/>
       <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69" s="7"/>
-      <c r="I69"/>
-    </row>
-    <row r="70" spans="1:9">
+      <c r="G69" s="7"/>
+      <c r="H69"/>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
       <c r="E70"/>
       <c r="F70"/>
-      <c r="G70"/>
-      <c r="H70" s="7"/>
-      <c r="I70"/>
-    </row>
-    <row r="71" spans="1:9">
+      <c r="G70" s="7"/>
+      <c r="H70"/>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
       <c r="E71"/>
       <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71" s="7"/>
-      <c r="I71"/>
-    </row>
-    <row r="72" spans="1:9">
+      <c r="G71" s="7"/>
+      <c r="H71"/>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
       <c r="E72"/>
       <c r="F72"/>
-      <c r="G72"/>
-      <c r="H72" s="7"/>
-      <c r="I72"/>
-    </row>
-    <row r="73" spans="1:9">
+      <c r="G72" s="7"/>
+      <c r="H72"/>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
       <c r="E73"/>
       <c r="F73"/>
-      <c r="G73"/>
-      <c r="H73" s="7"/>
-      <c r="I73"/>
-    </row>
-    <row r="74" spans="1:9">
+      <c r="G73" s="7"/>
+      <c r="H73"/>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
       <c r="E74"/>
       <c r="F74"/>
-      <c r="G74"/>
-      <c r="H74" s="7"/>
-      <c r="I74"/>
-    </row>
-    <row r="75" spans="1:9">
+      <c r="G74" s="7"/>
+      <c r="H74"/>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
       <c r="E75"/>
       <c r="F75"/>
-      <c r="G75"/>
-      <c r="H75" s="7"/>
-      <c r="I75"/>
-    </row>
-    <row r="76" spans="1:9">
+      <c r="G75" s="7"/>
+      <c r="H75"/>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
       <c r="E76"/>
       <c r="F76"/>
-      <c r="G76"/>
-      <c r="H76" s="7"/>
-      <c r="I76"/>
-    </row>
-    <row r="77" spans="1:9">
+      <c r="G76" s="7"/>
+      <c r="H76"/>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
       <c r="E77"/>
       <c r="F77"/>
-      <c r="G77"/>
-      <c r="H77" s="7"/>
-      <c r="I77"/>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="G77" s="7"/>
+      <c r="H77"/>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
       <c r="E78"/>
       <c r="F78"/>
-      <c r="G78"/>
-      <c r="H78" s="7"/>
-      <c r="I78"/>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="G78" s="7"/>
+      <c r="H78"/>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
       <c r="E79"/>
       <c r="F79"/>
-      <c r="G79"/>
-      <c r="H79" s="7"/>
-      <c r="I79"/>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="G79" s="7"/>
+      <c r="H79"/>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
       <c r="E80"/>
       <c r="F80"/>
-      <c r="G80"/>
-      <c r="H80" s="7"/>
-      <c r="I80"/>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="G80" s="7"/>
+      <c r="H80"/>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
       <c r="E81"/>
       <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81" s="7"/>
-      <c r="I81"/>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="G81" s="7"/>
+      <c r="H81"/>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82"/>
       <c r="F82"/>
-      <c r="G82"/>
-      <c r="H82" s="7"/>
-      <c r="I82"/>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="G82" s="7"/>
+      <c r="H82"/>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
       <c r="E83"/>
       <c r="F83"/>
-      <c r="G83"/>
-      <c r="H83" s="7"/>
-      <c r="I83"/>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="G83" s="7"/>
+      <c r="H83"/>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
       <c r="E84"/>
       <c r="F84"/>
-      <c r="G84"/>
-      <c r="H84" s="7"/>
-      <c r="I84"/>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="G84" s="7"/>
+      <c r="H84"/>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
       <c r="E85"/>
       <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85" s="7"/>
-      <c r="I85"/>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="G85" s="7"/>
+      <c r="H85"/>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
       <c r="E86"/>
       <c r="F86"/>
-      <c r="G86"/>
-      <c r="H86" s="7"/>
-      <c r="I86"/>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="G86" s="7"/>
+      <c r="H86"/>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
       <c r="E87"/>
       <c r="F87"/>
-      <c r="G87"/>
-      <c r="H87" s="7"/>
-      <c r="I87"/>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="G87" s="7"/>
+      <c r="H87"/>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
       <c r="E88"/>
       <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88" s="7"/>
-      <c r="I88"/>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="G88" s="7"/>
+      <c r="H88"/>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
       <c r="E89"/>
       <c r="F89"/>
-      <c r="G89"/>
-      <c r="H89" s="7"/>
-      <c r="I89"/>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="G89" s="7"/>
+      <c r="H89"/>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
       <c r="E90"/>
       <c r="F90"/>
-      <c r="G90"/>
-      <c r="H90" s="7"/>
-      <c r="I90"/>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="G90" s="7"/>
+      <c r="H90"/>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="11"/>
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
       <c r="E91"/>
       <c r="F91"/>
-      <c r="G91"/>
-      <c r="H91" s="7"/>
-      <c r="I91"/>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="G91" s="7"/>
+      <c r="H91"/>
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
       <c r="E92"/>
       <c r="F92"/>
-      <c r="G92"/>
-      <c r="H92" s="7"/>
-      <c r="I92"/>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="G92" s="7"/>
+      <c r="H92"/>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
       <c r="E93"/>
       <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93" s="7"/>
-      <c r="I93"/>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="G93" s="7"/>
+      <c r="H93"/>
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
       <c r="E94"/>
       <c r="F94"/>
-      <c r="G94"/>
-      <c r="H94" s="7"/>
-      <c r="I94"/>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="G94" s="7"/>
+      <c r="H94"/>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
       <c r="D95"/>
       <c r="E95"/>
       <c r="F95"/>
-      <c r="G95"/>
-      <c r="H95" s="7"/>
-      <c r="I95"/>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="G95" s="7"/>
+      <c r="H95"/>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
       <c r="D96"/>
       <c r="E96"/>
       <c r="F96"/>
-      <c r="G96"/>
-      <c r="H96" s="7"/>
-      <c r="I96"/>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="G96" s="7"/>
+      <c r="H96"/>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
       <c r="D97"/>
       <c r="E97"/>
       <c r="F97"/>
-      <c r="G97"/>
-      <c r="H97" s="7"/>
-      <c r="I97"/>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="G97" s="7"/>
+      <c r="H97"/>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
       <c r="D98"/>
       <c r="E98"/>
       <c r="F98"/>
-      <c r="G98"/>
-      <c r="H98" s="7"/>
-      <c r="I98"/>
-    </row>
-    <row r="99" spans="1:9">
+      <c r="G98" s="7"/>
+      <c r="H98"/>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
       <c r="D99"/>
       <c r="E99"/>
       <c r="F99"/>
-      <c r="G99"/>
-      <c r="H99" s="7"/>
-      <c r="I99"/>
-    </row>
-    <row r="100" spans="1:9">
+      <c r="G99" s="7"/>
+      <c r="H99"/>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
       <c r="D100"/>
       <c r="E100"/>
       <c r="F100"/>
-      <c r="G100"/>
-      <c r="H100" s="7"/>
-      <c r="I100"/>
-    </row>
-    <row r="101" spans="1:9">
+      <c r="G100" s="7"/>
+      <c r="H100"/>
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
       <c r="D101"/>
       <c r="E101"/>
       <c r="F101"/>
-      <c r="G101"/>
-      <c r="H101" s="7"/>
-      <c r="I101"/>
-    </row>
-    <row r="102" spans="1:9">
+      <c r="G101" s="7"/>
+      <c r="H101"/>
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
       <c r="D102"/>
       <c r="E102"/>
       <c r="F102"/>
-      <c r="G102"/>
-      <c r="H102" s="7"/>
-      <c r="I102"/>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="G102" s="7"/>
+      <c r="H102"/>
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
       <c r="D103"/>
       <c r="E103"/>
       <c r="F103"/>
-      <c r="G103"/>
-      <c r="H103" s="7"/>
-      <c r="I103"/>
-    </row>
-    <row r="104" spans="1:9">
+      <c r="G103" s="7"/>
+      <c r="H103"/>
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
       <c r="D104"/>
       <c r="E104"/>
       <c r="F104"/>
-      <c r="G104"/>
-      <c r="H104" s="7"/>
-      <c r="I104"/>
-    </row>
-    <row r="105" spans="1:9">
+      <c r="G104" s="7"/>
+      <c r="H104"/>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
       <c r="D105"/>
       <c r="E105"/>
       <c r="F105"/>
-      <c r="G105"/>
-      <c r="H105" s="7"/>
-      <c r="I105"/>
-    </row>
-    <row r="106" spans="1:9">
+      <c r="G105" s="7"/>
+      <c r="H105"/>
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
       <c r="D106"/>
       <c r="E106"/>
       <c r="F106"/>
-      <c r="G106"/>
-      <c r="H106" s="7"/>
-      <c r="I106"/>
-    </row>
-    <row r="107" spans="1:9">
+      <c r="G106" s="7"/>
+      <c r="H106"/>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
       <c r="D107"/>
       <c r="E107"/>
       <c r="F107"/>
-      <c r="G107"/>
-      <c r="H107" s="7"/>
-      <c r="I107"/>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="G107" s="7"/>
+      <c r="H107"/>
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
       <c r="D108"/>
       <c r="E108"/>
       <c r="F108"/>
-      <c r="G108"/>
-      <c r="H108" s="7"/>
-      <c r="I108"/>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="G108" s="7"/>
+      <c r="H108"/>
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
       <c r="D109"/>
       <c r="E109"/>
       <c r="F109"/>
-      <c r="G109"/>
-      <c r="H109" s="7"/>
-      <c r="I109"/>
-    </row>
-    <row r="110" spans="1:9">
+      <c r="G109" s="7"/>
+      <c r="H109"/>
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
       <c r="D110"/>
       <c r="E110"/>
       <c r="F110"/>
-      <c r="G110"/>
-      <c r="H110" s="7"/>
-      <c r="I110"/>
-    </row>
-    <row r="111" spans="1:9">
+      <c r="G110" s="7"/>
+      <c r="H110"/>
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
       <c r="D111"/>
       <c r="E111"/>
       <c r="F111"/>
-      <c r="G111"/>
-      <c r="H111" s="7"/>
-      <c r="I111"/>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="G111" s="7"/>
+      <c r="H111"/>
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
       <c r="D112"/>
       <c r="E112"/>
       <c r="F112"/>
-      <c r="G112"/>
-      <c r="H112" s="7"/>
-      <c r="I112"/>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="G112" s="7"/>
+      <c r="H112"/>
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113"/>
       <c r="B113"/>
       <c r="C113"/>
       <c r="D113"/>
       <c r="E113"/>
       <c r="F113"/>
-      <c r="G113"/>
-      <c r="H113" s="13"/>
-      <c r="I113"/>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="G113" s="13"/>
+      <c r="H113"/>
+    </row>
+    <row r="114" spans="1:8">
       <c r="A114"/>
       <c r="B114"/>
       <c r="C114"/>
       <c r="D114"/>
       <c r="E114"/>
       <c r="F114"/>
-      <c r="G114"/>
-      <c r="H114" s="13"/>
-      <c r="I114"/>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="G114" s="13"/>
+      <c r="H114"/>
+    </row>
+    <row r="115" spans="1:8">
       <c r="A115"/>
       <c r="B115"/>
       <c r="C115"/>
       <c r="D115"/>
       <c r="E115"/>
       <c r="F115"/>
-      <c r="G115"/>
-      <c r="H115" s="13"/>
-      <c r="I115"/>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="G115" s="13"/>
+      <c r="H115"/>
+    </row>
+    <row r="116" spans="1:8">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
       <c r="D116"/>
       <c r="E116"/>
       <c r="F116"/>
-      <c r="G116"/>
-      <c r="H116" s="13"/>
-      <c r="I116"/>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="G116" s="13"/>
+      <c r="H116"/>
+    </row>
+    <row r="117" spans="1:8">
       <c r="A117"/>
       <c r="B117"/>
       <c r="C117"/>
       <c r="D117"/>
       <c r="E117"/>
       <c r="F117"/>
-      <c r="G117"/>
-      <c r="H117" s="13"/>
-      <c r="I117"/>
-    </row>
-    <row r="118" spans="1:9">
+      <c r="G117" s="13"/>
+      <c r="H117"/>
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118"/>
       <c r="B118"/>
       <c r="C118"/>
@@ -3373,130 +3221,118 @@
       <c r="F118"/>
       <c r="G118"/>
       <c r="H118"/>
-      <c r="I118"/>
-    </row>
-    <row r="119" spans="1:9">
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119"/>
       <c r="B119"/>
       <c r="C119"/>
       <c r="D119"/>
       <c r="E119"/>
       <c r="F119"/>
-      <c r="G119"/>
-      <c r="H119" s="13"/>
-      <c r="I119"/>
-    </row>
-    <row r="120" spans="1:9">
+      <c r="G119" s="13"/>
+      <c r="H119"/>
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120"/>
       <c r="B120"/>
       <c r="C120"/>
       <c r="D120"/>
       <c r="E120"/>
       <c r="F120"/>
-      <c r="G120"/>
-      <c r="H120" s="13"/>
-      <c r="I120"/>
-    </row>
-    <row r="121" spans="1:9">
+      <c r="G120" s="13"/>
+      <c r="H120"/>
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121"/>
       <c r="B121"/>
       <c r="C121"/>
       <c r="D121"/>
       <c r="E121"/>
       <c r="F121"/>
-      <c r="G121"/>
-      <c r="H121" s="13"/>
-      <c r="I121"/>
-    </row>
-    <row r="122" spans="1:9">
+      <c r="G121" s="13"/>
+      <c r="H121"/>
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122"/>
       <c r="B122"/>
       <c r="C122"/>
       <c r="D122"/>
       <c r="E122"/>
       <c r="F122"/>
-      <c r="G122"/>
-      <c r="H122" s="13"/>
-      <c r="I122"/>
-    </row>
-    <row r="123" spans="1:9">
+      <c r="G122" s="13"/>
+      <c r="H122"/>
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123"/>
       <c r="B123"/>
       <c r="C123"/>
       <c r="D123"/>
       <c r="E123"/>
       <c r="F123"/>
-      <c r="G123"/>
-      <c r="H123" s="13"/>
-      <c r="I123"/>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="G123" s="13"/>
+      <c r="H123"/>
+    </row>
+    <row r="124" spans="1:8">
       <c r="A124"/>
       <c r="B124"/>
       <c r="C124"/>
       <c r="D124"/>
       <c r="E124"/>
       <c r="F124"/>
-      <c r="G124"/>
-      <c r="H124" s="13"/>
-      <c r="I124"/>
-    </row>
-    <row r="125" spans="1:9">
+      <c r="G124" s="13"/>
+      <c r="H124"/>
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125"/>
       <c r="B125"/>
       <c r="C125"/>
       <c r="D125"/>
       <c r="E125"/>
       <c r="F125"/>
-      <c r="G125"/>
-      <c r="H125" s="13"/>
-      <c r="I125"/>
-    </row>
-    <row r="126" spans="1:9">
+      <c r="G125" s="13"/>
+      <c r="H125"/>
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126"/>
       <c r="B126"/>
       <c r="C126"/>
       <c r="D126"/>
       <c r="E126"/>
       <c r="F126"/>
-      <c r="G126"/>
-      <c r="H126" s="13"/>
-      <c r="I126"/>
-    </row>
-    <row r="127" spans="1:9">
+      <c r="G126" s="13"/>
+      <c r="H126"/>
+    </row>
+    <row r="127" spans="1:8">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127"/>
       <c r="D127"/>
       <c r="E127"/>
       <c r="F127"/>
-      <c r="G127"/>
-      <c r="H127" s="13"/>
-      <c r="I127"/>
-    </row>
-    <row r="128" spans="1:9">
+      <c r="G127" s="13"/>
+      <c r="H127"/>
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128"/>
       <c r="B128"/>
       <c r="C128"/>
       <c r="D128"/>
       <c r="E128"/>
       <c r="F128"/>
-      <c r="G128"/>
-      <c r="H128" s="13"/>
-      <c r="I128"/>
-    </row>
-    <row r="129" spans="1:9">
+      <c r="G128" s="13"/>
+      <c r="H128"/>
+    </row>
+    <row r="129" spans="1:8">
       <c r="A129"/>
       <c r="B129"/>
       <c r="C129"/>
       <c r="D129"/>
       <c r="E129"/>
       <c r="F129"/>
-      <c r="G129"/>
-      <c r="H129" s="13"/>
-      <c r="I129"/>
-    </row>
-    <row r="130" spans="1:9">
+      <c r="G129" s="13"/>
+      <c r="H129"/>
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130"/>
       <c r="B130"/>
       <c r="C130"/>
@@ -3505,20 +3341,18 @@
       <c r="F130"/>
       <c r="G130"/>
       <c r="H130"/>
-      <c r="I130"/>
-    </row>
-    <row r="131" spans="1:9">
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131"/>
       <c r="B131"/>
       <c r="C131"/>
       <c r="D131"/>
       <c r="E131"/>
       <c r="F131"/>
-      <c r="G131"/>
-      <c r="H131" s="13"/>
-      <c r="I131"/>
-    </row>
-    <row r="132" spans="1:9">
+      <c r="G131" s="13"/>
+      <c r="H131"/>
+    </row>
+    <row r="132" spans="1:8">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -3527,20 +3361,18 @@
       <c r="F132"/>
       <c r="G132"/>
       <c r="H132"/>
-      <c r="I132"/>
-    </row>
-    <row r="133" spans="1:9">
+    </row>
+    <row r="133" spans="1:8">
       <c r="A133"/>
       <c r="B133"/>
       <c r="C133"/>
       <c r="D133"/>
       <c r="E133"/>
       <c r="F133"/>
-      <c r="G133"/>
-      <c r="H133" s="13"/>
-      <c r="I133"/>
-    </row>
-    <row r="134" spans="1:9">
+      <c r="G133" s="13"/>
+      <c r="H133"/>
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134"/>
       <c r="B134"/>
       <c r="C134"/>
@@ -3549,9 +3381,8 @@
       <c r="F134"/>
       <c r="G134"/>
       <c r="H134"/>
-      <c r="I134"/>
-    </row>
-    <row r="135" spans="1:9">
+    </row>
+    <row r="135" spans="1:8">
       <c r="A135"/>
       <c r="B135"/>
       <c r="C135"/>
@@ -3560,262 +3391,261 @@
       <c r="F135"/>
       <c r="G135"/>
       <c r="H135"/>
-      <c r="I135"/>
-    </row>
-    <row r="136" spans="1:9">
+    </row>
+    <row r="136" spans="1:8">
       <c r="C136" s="4"/>
-      <c r="H136" s="14"/>
-    </row>
-    <row r="137" spans="1:9">
+      <c r="G136" s="14"/>
+    </row>
+    <row r="137" spans="1:8">
       <c r="C137" s="4"/>
-      <c r="H137" s="14"/>
-    </row>
-    <row r="138" spans="1:9">
+      <c r="G137" s="14"/>
+    </row>
+    <row r="138" spans="1:8">
       <c r="C138" s="4"/>
-      <c r="H138" s="14"/>
-    </row>
-    <row r="139" spans="1:9">
+      <c r="G138" s="14"/>
+    </row>
+    <row r="139" spans="1:8">
       <c r="C139" s="4"/>
-      <c r="H139" s="14"/>
-    </row>
-    <row r="140" spans="1:9">
+      <c r="G139" s="14"/>
+    </row>
+    <row r="140" spans="1:8">
       <c r="C140" s="4"/>
-      <c r="H140" s="14"/>
-    </row>
-    <row r="141" spans="1:9">
+      <c r="G140" s="14"/>
+    </row>
+    <row r="141" spans="1:8">
       <c r="C141" s="4"/>
-      <c r="H141" s="14"/>
-    </row>
-    <row r="142" spans="1:9">
+      <c r="G141" s="14"/>
+    </row>
+    <row r="142" spans="1:8">
       <c r="C142" s="4"/>
-      <c r="H142" s="14"/>
-    </row>
-    <row r="143" spans="1:9">
+      <c r="G142" s="14"/>
+    </row>
+    <row r="143" spans="1:8">
       <c r="C143" s="4"/>
-      <c r="H143" s="14"/>
-    </row>
-    <row r="144" spans="1:9">
+      <c r="G143" s="14"/>
+    </row>
+    <row r="144" spans="1:8">
       <c r="C144" s="4"/>
-      <c r="H144" s="14"/>
-    </row>
-    <row r="145" spans="3:8">
+      <c r="G144" s="14"/>
+    </row>
+    <row r="145" spans="3:7">
       <c r="C145" s="4"/>
-      <c r="H145" s="14"/>
-    </row>
-    <row r="146" spans="3:8">
+      <c r="G145" s="14"/>
+    </row>
+    <row r="146" spans="3:7">
       <c r="C146" s="4"/>
-      <c r="H146" s="14"/>
-    </row>
-    <row r="147" spans="3:8">
+      <c r="G146" s="14"/>
+    </row>
+    <row r="147" spans="3:7">
       <c r="C147" s="4"/>
-      <c r="H147" s="14"/>
-    </row>
-    <row r="148" spans="3:8">
+      <c r="G147" s="14"/>
+    </row>
+    <row r="148" spans="3:7">
       <c r="C148" s="4"/>
-      <c r="H148" s="14"/>
-    </row>
-    <row r="149" spans="3:8">
+      <c r="G148" s="14"/>
+    </row>
+    <row r="149" spans="3:7">
       <c r="C149" s="4"/>
     </row>
-    <row r="150" spans="3:8">
+    <row r="150" spans="3:7">
       <c r="C150" s="4"/>
     </row>
-    <row r="151" spans="3:8">
+    <row r="151" spans="3:7">
       <c r="C151" s="4"/>
     </row>
-    <row r="152" spans="3:8">
+    <row r="152" spans="3:7">
       <c r="C152" s="4"/>
     </row>
-    <row r="153" spans="3:8">
+    <row r="153" spans="3:7">
       <c r="C153" s="4"/>
     </row>
-    <row r="154" spans="3:8">
+    <row r="154" spans="3:7">
       <c r="C154" s="4"/>
     </row>
-    <row r="155" spans="3:8">
+    <row r="155" spans="3:7">
       <c r="C155" s="4"/>
     </row>
-    <row r="156" spans="3:8">
+    <row r="156" spans="3:7">
       <c r="C156" s="4"/>
     </row>
-    <row r="157" spans="3:8">
+    <row r="157" spans="3:7">
       <c r="C157" s="4"/>
     </row>
-    <row r="158" spans="3:8">
+    <row r="158" spans="3:7">
       <c r="C158" s="4"/>
     </row>
-    <row r="159" spans="3:8">
+    <row r="159" spans="3:7">
       <c r="C159" s="4"/>
     </row>
-    <row r="160" spans="3:8">
+    <row r="160" spans="3:7">
       <c r="C160" s="4"/>
     </row>
-    <row r="161" spans="3:8">
+    <row r="161" spans="3:7">
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="3:8">
+    <row r="162" spans="3:7">
       <c r="C162" s="4"/>
-      <c r="H162" s="2"/>
-    </row>
-    <row r="163" spans="3:8">
+      <c r="G162" s="2"/>
+    </row>
+    <row r="163" spans="3:7">
       <c r="C163" s="4"/>
-      <c r="H163" s="2"/>
-    </row>
-    <row r="164" spans="3:8">
+      <c r="G163" s="2"/>
+    </row>
+    <row r="164" spans="3:7">
       <c r="C164" s="4"/>
-      <c r="H164" s="2"/>
-    </row>
-    <row r="165" spans="3:8">
+      <c r="G164" s="2"/>
+    </row>
+    <row r="165" spans="3:7">
       <c r="C165" s="4"/>
-      <c r="H165" s="2"/>
-    </row>
-    <row r="167" spans="3:8">
+      <c r="G165" s="2"/>
+    </row>
+    <row r="167" spans="3:7">
       <c r="C167" s="4"/>
-      <c r="H167" s="2"/>
-    </row>
-    <row r="168" spans="3:8">
+      <c r="G167" s="2"/>
+    </row>
+    <row r="168" spans="3:7">
       <c r="C168" s="4"/>
-      <c r="H168" s="2"/>
-    </row>
-    <row r="169" spans="3:8">
+      <c r="G168" s="2"/>
+    </row>
+    <row r="169" spans="3:7">
       <c r="C169" s="4"/>
-      <c r="H169" s="2"/>
-    </row>
-    <row r="170" spans="3:8">
+      <c r="G169" s="2"/>
+    </row>
+    <row r="170" spans="3:7">
       <c r="C170" s="4"/>
-      <c r="H170" s="2"/>
-    </row>
-    <row r="171" spans="3:8">
+      <c r="G170" s="2"/>
+    </row>
+    <row r="171" spans="3:7">
       <c r="C171" s="4"/>
-      <c r="H171" s="2"/>
-    </row>
-    <row r="172" spans="3:8">
+      <c r="G171" s="2"/>
+    </row>
+    <row r="172" spans="3:7">
       <c r="C172" s="4"/>
-      <c r="H172" s="2"/>
-    </row>
-    <row r="173" spans="3:8">
+      <c r="G172" s="2"/>
+    </row>
+    <row r="173" spans="3:7">
       <c r="C173" s="4"/>
-      <c r="H173" s="2"/>
-    </row>
-    <row r="174" spans="3:8">
+      <c r="G173" s="2"/>
+    </row>
+    <row r="174" spans="3:7">
       <c r="C174" s="4"/>
-      <c r="H174" s="2"/>
-    </row>
-    <row r="175" spans="3:8">
+      <c r="G174" s="2"/>
+    </row>
+    <row r="175" spans="3:7">
       <c r="C175" s="4"/>
-      <c r="H175" s="2"/>
-    </row>
-    <row r="176" spans="3:8">
+      <c r="G175" s="2"/>
+    </row>
+    <row r="176" spans="3:7">
       <c r="C176" s="4"/>
-      <c r="H176" s="2"/>
-    </row>
-    <row r="177" spans="3:8">
+      <c r="G176" s="2"/>
+    </row>
+    <row r="177" spans="3:7">
       <c r="C177" s="4"/>
-      <c r="H177" s="2"/>
-    </row>
-    <row r="178" spans="3:8">
+      <c r="G177" s="2"/>
+    </row>
+    <row r="178" spans="3:7">
       <c r="C178" s="4"/>
-      <c r="H178" s="2"/>
-    </row>
-    <row r="179" spans="3:8">
+      <c r="G178" s="2"/>
+    </row>
+    <row r="179" spans="3:7">
       <c r="C179" s="4"/>
-      <c r="H179" s="2"/>
-    </row>
-    <row r="180" spans="3:8">
+      <c r="G179" s="2"/>
+    </row>
+    <row r="180" spans="3:7">
       <c r="C180" s="4"/>
-      <c r="H180" s="2"/>
-    </row>
-    <row r="181" spans="3:8">
+      <c r="G180" s="2"/>
+    </row>
+    <row r="181" spans="3:7">
       <c r="C181" s="4"/>
-      <c r="H181" s="2"/>
-    </row>
-    <row r="182" spans="3:8">
+      <c r="G181" s="2"/>
+    </row>
+    <row r="182" spans="3:7">
       <c r="C182" s="4"/>
-      <c r="H182" s="2"/>
-    </row>
-    <row r="183" spans="3:8">
+      <c r="G182" s="2"/>
+    </row>
+    <row r="183" spans="3:7">
       <c r="C183" s="4"/>
-      <c r="H183" s="2"/>
-    </row>
-    <row r="184" spans="3:8">
+      <c r="G183" s="2"/>
+    </row>
+    <row r="184" spans="3:7">
       <c r="C184" s="4"/>
-      <c r="H184" s="2"/>
-    </row>
-    <row r="185" spans="3:8">
+      <c r="G184" s="2"/>
+    </row>
+    <row r="185" spans="3:7">
       <c r="C185" s="4"/>
-      <c r="H185" s="2"/>
-    </row>
-    <row r="186" spans="3:8">
+      <c r="G185" s="2"/>
+    </row>
+    <row r="186" spans="3:7">
       <c r="C186" s="4"/>
-      <c r="H186" s="2"/>
-    </row>
-    <row r="187" spans="3:8">
+      <c r="G186" s="2"/>
+    </row>
+    <row r="187" spans="3:7">
       <c r="C187" s="4"/>
-      <c r="H187" s="2"/>
-    </row>
-    <row r="188" spans="3:8">
+      <c r="G187" s="2"/>
+    </row>
+    <row r="188" spans="3:7">
       <c r="C188" s="4"/>
-      <c r="H188" s="2"/>
-    </row>
-    <row r="189" spans="3:8">
+      <c r="G188" s="2"/>
+    </row>
+    <row r="189" spans="3:7">
       <c r="C189" s="4"/>
-      <c r="H189" s="2"/>
-    </row>
-    <row r="190" spans="3:8">
+      <c r="G189" s="2"/>
+    </row>
+    <row r="190" spans="3:7">
       <c r="C190" s="4"/>
-      <c r="H190" s="2"/>
-    </row>
-    <row r="191" spans="3:8">
+      <c r="G190" s="2"/>
+    </row>
+    <row r="191" spans="3:7">
       <c r="C191" s="4"/>
-      <c r="H191" s="2"/>
-    </row>
-    <row r="192" spans="3:8">
+      <c r="G191" s="2"/>
+    </row>
+    <row r="192" spans="3:7">
       <c r="C192" s="4"/>
-      <c r="H192" s="2"/>
-    </row>
-    <row r="193" spans="3:8">
+      <c r="G192" s="2"/>
+    </row>
+    <row r="193" spans="3:7">
       <c r="C193" s="4"/>
-      <c r="H193" s="2"/>
-    </row>
-    <row r="194" spans="3:8">
+      <c r="G193" s="2"/>
+    </row>
+    <row r="194" spans="3:7">
       <c r="C194" s="4"/>
-      <c r="H194" s="2"/>
-    </row>
-    <row r="195" spans="3:8">
+      <c r="G194" s="2"/>
+    </row>
+    <row r="195" spans="3:7">
       <c r="C195" s="4"/>
-      <c r="H195" s="2"/>
-    </row>
-    <row r="196" spans="3:8">
+      <c r="G195" s="2"/>
+    </row>
+    <row r="196" spans="3:7">
       <c r="C196" s="4"/>
-      <c r="H196" s="2"/>
-    </row>
-    <row r="197" spans="3:8">
+      <c r="G196" s="2"/>
+    </row>
+    <row r="197" spans="3:7">
       <c r="C197" s="4"/>
-      <c r="H197" s="2"/>
-    </row>
-    <row r="198" spans="3:8">
+      <c r="G197" s="2"/>
+    </row>
+    <row r="198" spans="3:7">
       <c r="C198" s="4"/>
-      <c r="H198" s="2"/>
-    </row>
-    <row r="199" spans="3:8">
+      <c r="G198" s="2"/>
+    </row>
+    <row r="199" spans="3:7">
       <c r="C199" s="4"/>
-      <c r="H199" s="2"/>
-    </row>
-    <row r="200" spans="3:8">
+      <c r="G199" s="2"/>
+    </row>
+    <row r="200" spans="3:7">
       <c r="C200" s="4"/>
-      <c r="H200" s="2"/>
-    </row>
-    <row r="201" spans="3:8">
+      <c r="G200" s="2"/>
+    </row>
+    <row r="201" spans="3:7">
       <c r="C201" s="4"/>
-      <c r="H201" s="2"/>
-    </row>
-    <row r="202" spans="3:8">
+      <c r="G201" s="2"/>
+    </row>
+    <row r="202" spans="3:7">
       <c r="C202" s="4"/>
-      <c r="H202" s="2"/>
-    </row>
-    <row r="203" spans="3:8">
+      <c r="G202" s="2"/>
+    </row>
+    <row r="203" spans="3:7">
       <c r="C203" s="4"/>
-      <c r="H203" s="2"/>
+      <c r="G203" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3828,7 +3658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>